<commit_message>
resultat au bd et filtrage
</commit_message>
<xml_diff>
--- a/exported_data.xlsx
+++ b/exported_data.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,36 +440,73 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Contenu</t>
+          <t>Maladies</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Maladies</t>
+          <t>Résumés</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Résumés</t>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Pays</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>['Four Texas horses positive for EIA Four horses in Texas have been confirmed positive for equine infectious anemia (EIA). The cases are located in Waller, Montgomery, Denton and El Paso counties.\n\nAll four horses were Quarter Horses and have been euthanized. The Texas Animal Health Commission is working closely with the owners and local veterinarians to monitor potentially exposed horses.\n\nEDCC Health Watch is an Equine Network marketing program that utilizes information from the Equine Disease Communication Center (EDCC) to create and disseminate verified equine disease reports. The EDCC is an independent nonprofit organization that is supported by industry donations in order to provide open access to infectious disease information.\n\nAbout EIA\n\nEquine infectious anemia is a viral disease that attacks horses’ immune systems. The virus is transmitted through the exchange of body fluids from an infected to an uninfected animal, often by blood-feeding insects such as horseflies. It can also be transmitted through the use of blood-contaminated instruments or needles.\n\nA Coggins test screens horses’ blood for antibodies that are indicative of the presence of the EIA virus. Most U.S. states require horses to have proof of a negative Coggins test to travel across state lines.\n\nOnce an animal is infected with EIA, it is infected for life and can be a reservoir for the spread of disease. Not all horses show signs of disease, but those that do can exhibit:\n\nProgressive body condition loss;\n\nMuscle weakness;\n\nPoor stamina;\n\nFever;\n\nDepression; and\n\nAnemia.\n\nEIA has no vaccine and no cure. A horse diagnosed with the disease dies, is euthanized or must be placed under extremely strict quarantine conditions (at least 200 yards away from unaffected equids) for the rest of his life.']</t>
+          <t>tuberculose</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'equine infectious anemia'}</t>
+          <t>Tuberculose bovine : mesures renforcées face à la hausse des foyers Formation à la biosécurité, revalorisation des indemnisations, expérimentation d’un vaccin sur le blaireau, nouveau test de dépistage… Le ministère de l’Agriculture a mis en place différentes mesures de prévention pour endiguer la hausse du nombre de foyers de tuberculose bovine « dans plusieurs zones géographiques (Sud-Ouest, Normandie, Corse) et sa persistance dans d’autres (Côte d’Or, Camargue) », indique un communiqué du 5 avril. Cette maladie réglementée, transmissible à l’homme, peut être véhiculée par la faune sauvage. Les premiers tests du protocole de vaccination seront effectués en Nouvelle-Aquitaine, puis pourront être étendus « à l’ensemble des zones contaminées ». Le département, régulièrement concerné par des infections, est placé sous surveillance renforcée depuis 2015.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[{'summary_text': ' Four horses in Texas have been confirmed positive for equine infectious anemia . The cases are located in Waller  Montgomery  Denton and El Paso counties . All four horses were Quarter Horses and have been euthanized . The Texas Animal Health Commission is working closely with the owners and local veterinarians to monitor horses .'}]</t>
-        </is>
-      </c>
+          <t>https://urlz.fr/lEgR</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Calvados, France</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>الجلد العقدي</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>تعليمات عاجلة لوقف حركة نقل الأبقار بسبب اشتباه في مرض التهاب الجلد العقدي الوطن | رصد توجهت وزارة الزراعة والثروة الحيوانية بتعليمات عاجلة إلى المنسقين في قطاعات الزراعة والثروة الحيوانية بالبلديات، بناءً على التقارير الواردة حول اشتباه في إصابات بمرض التهاب الجلد العقدي في الأبقار. ونظرًا لنتائج العينات التي أظهرت إصابة بالمرض الفيروسي، طلبت الوزارة بشكل عاجل إبلاغ الجهات المختصة بوقف حركة نقل وتنقل الأبقار بين البلديات ومنع عرضها في أسواق المواشي حتى إشعار آخر. تأتي هذه الإجراءات تنفيذًا لقانون الوقاية من الأمراض الحيوانية المعدية، وتهدف إلى حماية الثروة الحيوانية ومنع انتشار المرض.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.libyaakhbar.com/libya-news/2263865.html</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>45239.7459375</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
filter date et restriction sur l'ajout
</commit_message>
<xml_diff>
--- a/exported_data.xlsx
+++ b/exported_data.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,46 +463,137 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tuberculose</t>
+          <t>equine encephalomyelitis</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Tuberculose bovine : mesures renforcées face à la hausse des foyers Formation à la biosécurité, revalorisation des indemnisations, expérimentation d’un vaccin sur le blaireau, nouveau test de dépistage… Le ministère de l’Agriculture a mis en place différentes mesures de prévention pour endiguer la hausse du nombre de foyers de tuberculose bovine « dans plusieurs zones géographiques (Sud-Ouest, Normandie, Corse) et sa persistance dans d’autres (Côte d’Or, Camargue) », indique un communiqué du 5 avril. Cette maladie réglementée, transmissible à l’homme, peut être véhiculée par la faune sauvage. Les premiers tests du protocole de vaccination seront effectués en Nouvelle-Aquitaine, puis pourront être étendus « à l’ensemble des zones contaminées ». Le département, régulièrement concerné par des infections, est placé sous surveillance renforcée depuis 2015.</t>
+          <t>Equine encephalomyelitis, Argentina declares sanitary emergency; Uruguay reports first case Equine encephalomyelitis, Argentina declares sanitary emergency; Uruguay reports first case Equine encephalomyelitis is highly contagious and can affect humans Argentina has finally declared a sanitary emergency in all of its territory, following an increase in equine encephalomyelitis, EE, and anticipates immediate, extraordinary, exceptional measures to contain further outbreaks of the virus disease. The Argentine government points out that the East, West and Venezuelan variants of EE, are viral infections, transmitted by mosquitoes, which can cause very serious encephalitis in horses and eventually humans.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://urlz.fr/lEgR</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>https://en.mercopress.com/2023/12/04/equine-encephalomyelitis-argentina-declares-sanitary-emergency-uruguay-reports-first-case</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2023-12-04</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Calvados, France</t>
+          <t>Paysandu, Argentina</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>الجلد العقدي</t>
+          <t>equine encephalomyelitis</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>تعليمات عاجلة لوقف حركة نقل الأبقار بسبب اشتباه في مرض التهاب الجلد العقدي الوطن | رصد توجهت وزارة الزراعة والثروة الحيوانية بتعليمات عاجلة إلى المنسقين في قطاعات الزراعة والثروة الحيوانية بالبلديات، بناءً على التقارير الواردة حول اشتباه في إصابات بمرض التهاب الجلد العقدي في الأبقار. ونظرًا لنتائج العينات التي أظهرت إصابة بالمرض الفيروسي، طلبت الوزارة بشكل عاجل إبلاغ الجهات المختصة بوقف حركة نقل وتنقل الأبقار بين البلديات ومنع عرضها في أسواق المواشي حتى إشعار آخر. تأتي هذه الإجراءات تنفيذًا لقانون الوقاية من الأمراض الحيوانية المعدية، وتهدف إلى حماية الثروة الحيوانية ومنع انتشار المرض.</t>
+          <t>Equine encephalomyelitis, Argentina declares sanitary emergency; Uruguay reports first case Equine encephalomyelitis, Argentina declares sanitary emergency; Uruguay reports first case Equine encephalomyelitis is highly contagious and can affect humans Argentina has finally declared a sanitary emergency in all of its territory, following an increase in equine encephalomyelitis, EE, and anticipates immediate, extraordinary, exceptional measures to contain further outbreaks of the virus disease. The Argentine government points out that the East, West and Venezuelan variants of EE, are viral infections, transmitted by mosquitoes, which can cause very serious encephalitis in horses and eventually humans.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.libyaakhbar.com/libya-news/2263865.html</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>45239.7459375</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>https://en.mercopress.com/2023/12/04/equine-encephalomyelitis-argentina-declares-sanitary-emergency-uruguay-reports-first-case</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2023-12-04</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Paysandu, Argentina</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>bluetongue</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>But the disease has resurfaced this year and animal health experts reported that a new strain, named BTV-3, had been confirmed on more than 700 Dutch farms by early October - with a new case also reported in Belgium this week. “The existing BTV-8 serotype vaccine will not offer cross-protection against this new BTV-3 strain, making any likely outbreak difficult to control. "Hence why it’s so important that we follow the advice to take action and prioritise good biosecurity measures while remaining extremely vigilant to the disease at this stage." Dr Henry added: "It remains extremely difficult to protect against midges and a vector-borne disease.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://lc.cx/nLtrtC</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2023-10-11</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Belgium</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>brucellosis</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Brucellosis, a zoonotic disease caused by the bacterial genus Brucella, has been confirmed in two natives of Vembayam in Thiruvananthapuram. A statement issued by the Animal Husbandry department said that it was difficult to recognise the disease in animals, as it did not produce any overt symptoms in animals. The bacteria are transmitted from animals to humans by ingestion through infected food products, direct contact with an infected animal, or through the inhalation of aerosols. Minister for Animal Husbandry J. Chinchurani, said that apart from giving awareness classes to dairy farmers, the department would test milk samples from milk societies also.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://lc.cx/4H9k-A</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2023-10-09</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Thiruvananthapuram, Kerala, Kollam</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>west nile virus, eastern equine encephalitis</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>The first EEE positive mosquito pool was detected in Gloucester County this year (https://www.nj.gov/health/cd/statistics/arboviral-stats/). “Vaccinated animals are much less likely to contract deadly diseases such as EEE and West Nile Virus.” For more information about EEE in horses, visit the New Jersey Department of Agriculture website at: http://www.nj.gov/agriculture/divisions/ah/diseases/diseaseworksheets.html EEE and West Nile virus, like other viral diseases affecting a horse’s neurological system, must be reported to the state veterinarian at 609-671-6400 within 48 hours of diagnosis.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://lc.cx/RqYUj8</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2023-10-25</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>New Jersey, Gloucester County</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
exporter data dans filter
</commit_message>
<xml_diff>
--- a/exported_data.xlsx
+++ b/exported_data.xlsx
@@ -463,135 +463,135 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>equine encephalomyelitis</t>
+          <t>eastern equine encephalitis, west nile virus</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Equine encephalomyelitis, Argentina declares sanitary emergency; Uruguay reports first case Equine encephalomyelitis, Argentina declares sanitary emergency; Uruguay reports first case Equine encephalomyelitis is highly contagious and can affect humans Argentina has finally declared a sanitary emergency in all of its territory, following an increase in equine encephalomyelitis, EE, and anticipates immediate, extraordinary, exceptional measures to contain further outbreaks of the virus disease. The Argentine government points out that the East, West and Venezuelan variants of EE, are viral infections, transmitted by mosquitoes, which can cause very serious encephalitis in horses and eventually humans.</t>
+          <t>The first EEE positive mosquito pool was detected in Gloucester County this year (https://www.nj.gov/health/cd/statistics/arboviral-stats/). “Vaccinated animals are much less likely to contract deadly diseases such as EEE and West Nile Virus.” For more information about EEE in horses, visit the New Jersey Department of Agriculture website at: http://www.nj.gov/agriculture/divisions/ah/diseases/diseaseworksheets.html EEE and West Nile virus, like other viral diseases affecting a horse’s neurological system, must be reported to the state veterinarian at 609-671-6400 within 48 hours of diagnosis.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://en.mercopress.com/2023/12/04/equine-encephalomyelitis-argentina-declares-sanitary-emergency-uruguay-reports-first-case</t>
+          <t>https://lc.cx/RqYUj8</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023-12-04</t>
+          <t>2023-10-25</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Paysandu, Argentina</t>
+          <t>New Jersey, Gloucester County</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>equine encephalomyelitis</t>
+          <t>bluetongue</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Equine encephalomyelitis, Argentina declares sanitary emergency; Uruguay reports first case Equine encephalomyelitis, Argentina declares sanitary emergency; Uruguay reports first case Equine encephalomyelitis is highly contagious and can affect humans Argentina has finally declared a sanitary emergency in all of its territory, following an increase in equine encephalomyelitis, EE, and anticipates immediate, extraordinary, exceptional measures to contain further outbreaks of the virus disease. The Argentine government points out that the East, West and Venezuelan variants of EE, are viral infections, transmitted by mosquitoes, which can cause very serious encephalitis in horses and eventually humans.</t>
+          <t>But the disease has resurfaced this year and animal health experts reported that a new strain, named BTV-3, had been confirmed on more than 700 Dutch farms by early October - with a new case also reported in Belgium this week. “The existing BTV-8 serotype vaccine will not offer cross-protection against this new BTV-3 strain, making any likely outbreak difficult to control. "Hence why it’s so important that we follow the advice to take action and prioritise good biosecurity measures while remaining extremely vigilant to the disease at this stage." Dr Henry added: "It remains extremely difficult to protect against midges and a vector-borne disease.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://en.mercopress.com/2023/12/04/equine-encephalomyelitis-argentina-declares-sanitary-emergency-uruguay-reports-first-case</t>
+          <t>https://lc.cx/nLtrtC</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2023-12-04</t>
+          <t>2023-10-11</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Paysandu, Argentina</t>
+          <t>Belgium</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>bluetongue</t>
+          <t>eastern equine encephalitis, west nile virus</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>But the disease has resurfaced this year and animal health experts reported that a new strain, named BTV-3, had been confirmed on more than 700 Dutch farms by early October - with a new case also reported in Belgium this week. “The existing BTV-8 serotype vaccine will not offer cross-protection against this new BTV-3 strain, making any likely outbreak difficult to control. "Hence why it’s so important that we follow the advice to take action and prioritise good biosecurity measures while remaining extremely vigilant to the disease at this stage." Dr Henry added: "It remains extremely difficult to protect against midges and a vector-borne disease.</t>
+          <t>The first EEE positive mosquito pool was detected in Gloucester County this year (https://www.nj.gov/health/cd/statistics/arboviral-stats/). “Vaccinated animals are much less likely to contract deadly diseases such as EEE and West Nile Virus.” For more information about EEE in horses, visit the New Jersey Department of Agriculture website at: http://www.nj.gov/agriculture/divisions/ah/diseases/diseaseworksheets.html EEE and West Nile virus, like other viral diseases affecting a horse’s neurological system, must be reported to the state veterinarian at 609-671-6400 within 48 hours of diagnosis.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://lc.cx/nLtrtC</t>
+          <t xml:space="preserve"> https://lc.cx/RqYUj8</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2023-10-11</t>
+          <t>2023-10-25</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>New Jersey, Gloucester County</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>brucellosis</t>
+          <t>fièvre aphteuse</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Brucellosis, a zoonotic disease caused by the bacterial genus Brucella, has been confirmed in two natives of Vembayam in Thiruvananthapuram. A statement issued by the Animal Husbandry department said that it was difficult to recognise the disease in animals, as it did not produce any overt symptoms in animals. The bacteria are transmitted from animals to humans by ingestion through infected food products, direct contact with an infected animal, or through the inhalation of aerosols. Minister for Animal Husbandry J. Chinchurani, said that apart from giving awareness classes to dairy farmers, the department would test milk samples from milk societies also.</t>
+          <t>Fièvre Aphteuse en Algérie : Une Campagne Préventive Cruciale pour Protéger le Cheptel National L’Algérie est en alerte face à une menace qui plane sur son secteur agricole. Les services vétérinaires sont mobilisés dans tout le pays pour garantir l’efficacité de la campagne. La fièvre aphteuse peut entraîner des pertes économiques considérables si elle n’est pas maîtrisée. Cependant, la riposte préventive par le biais d’une campagne de vaccination nationale démontre l’engagement du pays à protéger son cheptel national et à préserver son industrie agricole.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://lc.cx/4H9k-A</t>
+          <t>https://www.algerie-focus.com/fievre-aphteuse-en-algerie-une-campagne-preventive-cruciale-pour-proteger-le-cheptel-national/</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2023-10-09</t>
+          <t>2024-04-09</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Thiruvananthapuram, Kerala, Kollam</t>
+          <t>Algeria</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>west nile virus, eastern equine encephalitis</t>
+          <t>السل</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>The first EEE positive mosquito pool was detected in Gloucester County this year (https://www.nj.gov/health/cd/statistics/arboviral-stats/). “Vaccinated animals are much less likely to contract deadly diseases such as EEE and West Nile Virus.” For more information about EEE in horses, visit the New Jersey Department of Agriculture website at: http://www.nj.gov/agriculture/divisions/ah/diseases/diseaseworksheets.html EEE and West Nile virus, like other viral diseases affecting a horse’s neurological system, must be reported to the state veterinarian at 609-671-6400 within 48 hours of diagnosis.</t>
+          <t>كانت البداية بإعلان صحيفة محلية بيع 10 أبقار صادرة عن مركب فلاحي بسليانة شمال غربي تونس، مما أثار حفيظة عمادة البياطرة التي قالت إن الأبقار المعروضة للبيع مصابة بالسل، ودعا عميد الأطباء البياطرة أحمد رجب وزارة الفلاحة إلى التدخل من أجل إبطال عملية البيع، مما أعاد فتح ملف الأمراض الحيوانية التي تشكل خطراً على الإنسان. وقال رجب لـ"اندبندنت عربية" إن القانون رقم 95 لعام 2005 المتعلق بتربية الماشية والمنتجات الحيوانية في تونس يحظر على كل مالك أو مربي الاتجار بالحيوانات المصابة بأمراض مثل السل والأمراض شديدة العدوى التي تسبب خسائر اقتصادية ويمكن أن تنتقل من الحيوان إلى الإنسان، منوهاً بأن الأبقار المصابة بالسل لا تحمل علامات ويمكنها إطلاق جرثومة المرض في الحليب ومن ثم نقلها إلى البشر. يشار إلى أن تونس تعرف مئات الإصابات بالسل لدى البشر جراء انتقاله من الحيوان، وتصاعدت التحذيرات من أخطار صحية ناجمة عن انتشار السل الحيواني الذي يتسبب فيه استهلاك الألبان غير المعقمة أو الخاضعة للرقابة، وأسهم نقص الحليب المعلب في ارتفاع الإقبال على الحليب الخام الذي قد يهدد صحة الإنسان. يذكر أن مصالح وزارة الفلاحة في كل المحافظات تقدم سنوياً جدولاً زمنياً لتلقيح القطيع الحيواني لدى الخواص لمجابهة أمراض السل والكلب مجاناً.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://lc.cx/RqYUj8</t>
+          <t>https://lc.cx/GFQ2zw</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2023-10-25</t>
+          <t>2023-11-18</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>New Jersey, Gloucester County</t>
+          <t>Sulaylana, Tunisia, Baton</t>
         </is>
       </c>
     </row>

</xml_diff>